<commit_message>
button1_Click (fix enter failse PPhone) Add Form (Delete & Update)
</commit_message>
<xml_diff>
--- a/DuLieuMember.xlsx
+++ b/DuLieuMember.xlsx
@@ -24,48 +24,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>12AM-13PM</t>
-  </si>
-  <si>
-    <t>Khánh</t>
-  </si>
-  <si>
-    <t>7AM-8AM</t>
-  </si>
-  <si>
-    <t>CôngDaiKa</t>
-  </si>
-  <si>
-    <t>9AM-10PM</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>Phạm Hân</t>
-  </si>
-  <si>
-    <t>11AM-12PM</t>
-  </si>
-  <si>
-    <t>Hoàng Anh</t>
-  </si>
-  <si>
-    <t>1PM-2PM</t>
-  </si>
-  <si>
-    <t>Tiến</t>
-  </si>
-  <si>
-    <t>3PM-4PM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Emily Johnson</t>
+  </si>
+  <si>
+    <t>Michael Davis</t>
+  </si>
+  <si>
+    <t>Sarah Thompson</t>
+  </si>
+  <si>
+    <t>David Brown</t>
+  </si>
+  <si>
+    <t>Jennifer Wilson</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>6AM-8AM</t>
+  </si>
+  <si>
+    <t>8AM-10AM</t>
+  </si>
+  <si>
+    <t>6PM-8PM</t>
+  </si>
+  <si>
+    <t>8PM-10PM</t>
   </si>
 </sst>
 </file>
@@ -383,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G6"/>
+      <selection activeCell="A3" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,10 +393,10 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>2323223</v>
+        <v>12345</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1">
         <v>20</v>
@@ -411,7 +405,7 @@
         <v>2000</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -419,13 +413,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>26187</v>
+        <v>12346</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>18</v>
@@ -434,7 +428,7 @@
         <v>1000</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -442,10 +436,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>34322</v>
+        <v>12347</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -457,7 +451,7 @@
         <v>3000</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -465,10 +459,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>53453</v>
+        <v>12348</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -480,7 +474,7 @@
         <v>4000</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,13 +482,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>64544</v>
+        <v>12349</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>17</v>
@@ -511,13 +505,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>53434</v>
+        <v>12341</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>15</v>
@@ -526,7 +520,27 @@
         <v>500</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>